<commit_message>
Adding spreadsheets for YP-CORE
</commit_message>
<xml_diff>
--- a/docs/YP-CORE/YP-CORE1.xlsx
+++ b/docs/YP-CORE/YP-CORE1.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Current_share\Current_Data\MyR\shiny.psyctc.org\docs\YP-CORE\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FFFBF75-57D4-4D3E-8B10-22DC2E0020E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="13125" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Explanation" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Data" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Explanation" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -26,130 +31,114 @@
     <t xml:space="preserve">The second worksheet in this spreadsheet is intended to help create a dataset for analysis in apps at </t>
   </si>
   <si>
-    <t xml:space="preserve">https://shiny.psyctc.org/docs/YP-CORE/index.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It has nine columns but you can add as many as you like to the right of OtherVariable1, if you do, you must put the variable name in the first row of each of your additional columns</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The nine columns are fairly self-explanatory and have some minimal validity checking preventing input of at least some impossible values.  The variables are:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Column name (all names in row 1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Restrictions/validation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RespondentID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No restrictions on format or values but something must be entered</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Make sure you use a distinct value for each respondent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TherapistID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">None</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Make sure you use a distinct value for each therapist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Must be a valid date after 31/12/97 and before 31/12/2050, mandatory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SessionN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Must be an integer greater than zero, can be blank</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No restrictions and can be blank</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Must be an integer between 11 and 25 (inclusive), can be blank</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ypmean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Must be between 0 and 4 (inclusive)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YP-CORE score if mean scoring used</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ypscore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Must be between 0 and 40 (inclusive)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YP-CORE score if ‘clinical’ scoring used</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OtherVariable1</t>
+    <t>https://shiny.psyctc.org/docs/YP-CORE/index.html</t>
+  </si>
+  <si>
+    <t>It has nine columns but you can add as many as you like to the right of OtherVariable1, if you do, you must put the variable name in the first row of each of your additional columns</t>
+  </si>
+  <si>
+    <t>The nine columns are fairly self-explanatory and have some minimal validity checking preventing input of at least some impossible values.  The variables are:</t>
+  </si>
+  <si>
+    <t>Column name (all names in row 1)</t>
+  </si>
+  <si>
+    <t>Restrictions/validation</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>RespondentID</t>
+  </si>
+  <si>
+    <t>No restrictions on format or values but something must be entered</t>
+  </si>
+  <si>
+    <t>Make sure you use a distinct value for each respondent</t>
+  </si>
+  <si>
+    <t>TherapistID</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Make sure you use a distinct value for each therapist</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Must be a valid date after 31/12/97 and before 31/12/2050, mandatory</t>
+  </si>
+  <si>
+    <t>SessionN</t>
+  </si>
+  <si>
+    <t>Must be an integer greater than zero, can be blank</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>No restrictions and can be blank</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Must be an integer between 11 and 25 (inclusive), can be blank</t>
+  </si>
+  <si>
+    <t>Must be between 0 and 4 (inclusive)</t>
+  </si>
+  <si>
+    <t>YP-CORE score if mean scoring used</t>
+  </si>
+  <si>
+    <t>Must be between 0 and 40 (inclusive)</t>
+  </si>
+  <si>
+    <t>YP-CORE score if ‘clinical’ scoring used</t>
+  </si>
+  <si>
+    <t>OtherVariable1</t>
   </si>
   <si>
     <t xml:space="preserve">No restrictions </t>
   </si>
   <si>
-    <t xml:space="preserve">For the two columns where a value is mandatory the background colour is pale red until a valid value is entered when it turns pale green to show that something has been entered.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I have filled the first row with indicative values but you should delete those and start entering your own.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">On time, full session</t>
+    <t>For the two columns where a value is mandatory the background colour is pale red until a valid value is entered when it turns pale green to show that something has been entered.</t>
+  </si>
+  <si>
+    <t>I have filled the first row with indicative values but you should delete those and start entering your own.</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>On time, full session</t>
+  </si>
+  <si>
+    <t>YPmean</t>
+  </si>
+  <si>
+    <t>YPscore</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="13"/>
@@ -177,7 +166,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -185,62 +174,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF006600"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFCC0000"/>
@@ -250,7 +208,7 @@
           <bgColor rgb="FFFFCCCC"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
     </dxf>
     <dxf>
       <font>
@@ -261,9 +219,21 @@
           <bgColor rgb="FFCCFFCC"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCC0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -322,62 +292,78 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="LibreOffice">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="18a303"/>
+        <a:srgbClr val="18A303"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="0369a3"/>
+        <a:srgbClr val="0369A3"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="a33e03"/>
+        <a:srgbClr val="A33E03"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8e03a3"/>
+        <a:srgbClr val="8E03A3"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="c99c00"/>
+        <a:srgbClr val="C99C00"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="c9211e"/>
+        <a:srgbClr val="C9211E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000ee"/>
+        <a:srgbClr val="0000EE"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="551a8b"/>
+        <a:srgbClr val="551A8B"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="DejaVu Sans"/>
+        <a:cs typeface="DejaVu Sans"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="DejaVu Sans"/>
+        <a:cs typeface="DejaVu Sans"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme>
@@ -430,48 +416,47 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="16.15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="55.09"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="3" style="1" width="11.53"/>
+    <col min="1" max="1" width="29.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="55.140625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:3" s="2" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" s="2" customFormat="true" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:3" s="2" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -482,7 +467,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -493,7 +478,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -504,7 +489,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -512,7 +497,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -520,7 +505,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -528,7 +513,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -536,54 +521,53 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="1" t="s">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="1" t="s">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="1" t="s">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://shiny.psyctc.org/docs/YP-CORE/index.html"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -591,119 +575,115 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.63"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="n">
+      <c r="C2" s="4">
         <v>45798</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="0" t="n">
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2">
         <v>13</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2">
         <v>1.3</v>
       </c>
-      <c r="I2" s="0" t="s">
-        <v>32</v>
+      <c r="I2" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A1048576">
-    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>COUNTBLANK(A2) &gt; 0</formula>
     </cfRule>
-    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>COUNTBLANK(A2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C1048576">
-    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="expression" dxfId="1" priority="4">
       <formula>COUNTBLANK(C2) &gt; 0</formula>
     </cfRule>
-    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" dxfId="0" priority="5">
       <formula>COUNTBLANK(C2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="5">
-    <dataValidation allowBlank="true" error="Inadmissible date entered" errorStyle="stop" errorTitle="Inadmissible date" operator="between" promptTitle="Must be real date, e.g. 31/9/25 is not allowed" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C2:C1002" type="date">
+    <dataValidation type="date" allowBlank="1" showErrorMessage="1" errorTitle="Inadmissible date" error="Inadmissible date entered" promptTitle="Must be real date, e.g. 31/9/25 is not allowed" sqref="C2:C1002" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>35796</formula1>
       <formula2>55153</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Must be an integer greater than zero" errorStyle="stop" errorTitle="Impossible session number" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D2:D1002" type="whole">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showErrorMessage="1" errorTitle="Impossible session number" error="Must be an integer greater than zero" sqref="D2:D1002" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Must be a valid mean score, i.e. between 0 and 4" promptTitle="Must be a valid mean score" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2:G1002" type="decimal">
+    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" promptTitle="Must be a valid mean score" prompt="Must be a valid mean score, i.e. between 0 and 4" sqref="G2:G1002" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>0</formula1>
       <formula2>4</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Must be between 11 and 25 (inclusive)" errorStyle="stop" errorTitle="Inadmissible age" operator="between" prompt="Integer values between 11 and 25 (inclusive).  Referential data is not available above the age of 18 but the YP-CORE is used up to that age in some services for &quot;emerging adults&quot;" promptTitle="Age at last birthday" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F2:F1002" type="whole">
+    <dataValidation type="whole" allowBlank="1" showErrorMessage="1" errorTitle="Inadmissible age" error="Must be between 11 and 25 (inclusive)" promptTitle="Age at last birthday" prompt="Integer values between 11 and 25 (inclusive).  Referential data is not available above the age of 18 but the YP-CORE is used up to that age in some services for &quot;emerging adults&quot;" sqref="F2:F1002" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>11</formula1>
       <formula2>25</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Must be between 0 and 40" errorStyle="stop" errorTitle="Inadmissible score" operator="between" prompt="The 'clinical' score is 10x the mean item score" promptTitle="'Clinical' score: between 0 and 40" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2:H1002" type="decimal">
+    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="Inadmissible score" error="Must be between 0 and 40" promptTitle="'Clinical' score: between 0 and 40" prompt="The 'clinical' score is 10x the mean item score" sqref="H2:H1002" xr:uid="{00000000-0002-0000-0100-000004000000}">
       <formula1>0</formula1>
       <formula2>40</formula2>
     </dataValidation>
   </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>